<commit_message>
timetable system almost finished
</commit_message>
<xml_diff>
--- a/utils/example.xlsx
+++ b/utils/example.xlsx
@@ -558,7 +558,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -764,9 +764,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>970920</xdr:colOff>
+      <xdr:colOff>970560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>980280</xdr:rowOff>
+      <xdr:rowOff>979920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -780,7 +780,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11291400" cy="980280"/>
+          <a:ext cx="11296440" cy="979920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,10 +803,10 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>

</xml_diff>